<commit_message>
D7 new transverse tree
</commit_message>
<xml_diff>
--- a/output/results_old.xlsx
+++ b/output/results_old.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,32 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Fit time MeanSDTD5</t>
+          <t>Fit time sktree</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Prediction time MeanSDTD5</t>
+          <t>Prediction time sktree</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Score MeanSDTD5</t>
+          <t>Score sktree</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Fit time MeanSDTD6</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Prediction time MeanSDTD6</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Score MeanSDTD6</t>
         </is>
       </c>
     </row>
@@ -493,16 +508,25 @@
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01600265502929688</v>
+        <v>0.002012252807617188</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001996517181396484</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.01124763488769531</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="3">
@@ -523,16 +547,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02599811553955078</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.003998517990112305</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.9444444444444444</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.006361961364746094</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.01128768920898438</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="4">
@@ -553,16 +586,25 @@
         <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
-        <v>0.07899951934814453</v>
+        <v>0.01556801795959473</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01201796531677246</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8947368421052632</v>
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.02974939346313477</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.01807379722595215</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="5">
@@ -583,22 +625,31 @@
         <v>64</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4950032234191895</v>
+        <v>0.0401148796081543</v>
       </c>
       <c r="G5" t="n">
-        <v>0.05499744415283203</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6694444444444444</v>
+        <v>0.8527777777777777</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.09845972061157227</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.08024406433105469</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.7555555555555555</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Adult</t>
+          <t>BankNote Authentication</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -607,22 +658,109 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>48842</v>
+        <v>1372</v>
       </c>
       <c r="D6" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F6" t="n">
-        <v>144.9374601840973</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.037065744400024</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6425427372300133</v>
+        <v>0.9818181818181818</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04781126976013184</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.03228092193603516</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9636363636363636</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Gas Drift</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>13910</v>
+      </c>
+      <c r="D7" t="n">
+        <v>128</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.521384954452515</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.001997709274291992</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9410496046010065</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.5315756797790527</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.615117073059082</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Shuttle</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>classification</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>58000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1600716114044189</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9994827586206897</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1409909725189209</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.074449777603149</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9876724137931034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>